<commit_message>
fixing axiom exp. template
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Experiment_run_AXIOM_v4_6_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Experiment_run_AXIOM_v4_6_0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmarcelino/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0874F09E-B6C0-FB4F-AAC2-43A36E8F2E22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CFAA334-86FA-7A4D-B3DD-299AD19C9E9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3760" yWindow="-19260" windowWidth="27040" windowHeight="15780" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3460" yWindow="-21900" windowWidth="27040" windowHeight="15780" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Experiments" sheetId="1" r:id="rId1"/>
@@ -396,9 +396,6 @@
     <t>Auto-Loader</t>
   </si>
   <si>
-    <t>Tethys (GeneTitan)</t>
-  </si>
-  <si>
     <t>Nimbus 1</t>
   </si>
   <si>
@@ -414,9 +411,6 @@
     <t>On-Sequencer</t>
   </si>
   <si>
-    <t>Themis (GeneTitan)</t>
-  </si>
-  <si>
     <t>Nimbus 2</t>
   </si>
   <si>
@@ -1564,6 +1558,12 @@
   </si>
   <si>
     <t>P24</t>
+  </si>
+  <si>
+    <t>Protected (GeneTitan)</t>
+  </si>
+  <si>
+    <t>OnNetwork (GeneTitan)</t>
   </si>
 </sst>
 </file>
@@ -2250,9 +2250,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O996"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10326,15 +10326,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
-          <x14:formula1>
-            <xm:f>Index!$F$2:$F$4</xm:f>
-          </x14:formula1>
-          <x14:formula2>
-            <xm:f>0</xm:f>
-          </x14:formula2>
-          <xm:sqref>D7:D26</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>Index!$A$2:$A$3</xm:f>
@@ -10353,6 +10344,12 @@
           </x14:formula2>
           <xm:sqref>J15</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{4671A5B6-8819-4F46-BDA6-70684686855E}">
+          <x14:formula1>
+            <xm:f>Index!$F$2:$F$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>D7:D26</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -10363,7 +10360,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
@@ -18480,7 +18477,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+    <sheetView zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -20297,7 +20294,7 @@
   <dimension ref="A1:J1000"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20357,129 +20354,129 @@
       <c r="E2" t="s">
         <v>91</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="33" t="s">
+        <v>480</v>
+      </c>
+      <c r="G2" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="G2" s="31" t="s">
+      <c r="J2" t="s">
         <v>93</v>
-      </c>
-      <c r="J2" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" t="s">
         <v>95</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" t="s">
         <v>96</v>
       </c>
-      <c r="C3" t="s">
-        <v>96</v>
-      </c>
-      <c r="D3" t="s">
-        <v>96</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F3" s="33" t="s">
+        <v>481</v>
+      </c>
+      <c r="G3" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="F3" s="33" t="s">
+      <c r="J3" t="s">
         <v>98</v>
-      </c>
-      <c r="G3" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="J3" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D11" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D13" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
@@ -20487,100 +20484,100 @@
         <v>29</v>
       </c>
       <c r="D14" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D15" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D16" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D17" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D18" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C19" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D19" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="20" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C20" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D20" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="21" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C21" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D21" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C22" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D22" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="23" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C23" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D23" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="24" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D24" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="25" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D25" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="26" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C26" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D26" t="s">
         <v>29</v>
@@ -20591,196 +20588,196 @@
         <v>30</v>
       </c>
       <c r="D27" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C28" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D28" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="29" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C29" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D29" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="30" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C30" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D30" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C31" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D31" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="32" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C32" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D32" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="33" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C33" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D33" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="34" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C34" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D34" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="35" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C35" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D35" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="36" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D36" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="37" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C37" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D37" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="38" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C38" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D38" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="39" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C39" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D39" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="40" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C40" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D40" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="41" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C41" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D41" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="42" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C42" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D42" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="43" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C43" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D43" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="44" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C44" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D44" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="45" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C45" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D45" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="46" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C46" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D46" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="47" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C47" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D47" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="48" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C48" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D48" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="49" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C49" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D49" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="50" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C50" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D50" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="51" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C51" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D51" t="s">
         <v>30</v>
@@ -20788,1810 +20785,1810 @@
     </row>
     <row r="52" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C52" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D52" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="53" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C53" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D53" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="54" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C54" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D54" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="55" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C55" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D55" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="56" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C56" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D56" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="57" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C57" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D57" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="58" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C58" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D58" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="59" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C59" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D59" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="60" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C60" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D60" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="61" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C61" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D61" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="62" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C62" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D62" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="63" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C63" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D63" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="64" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C64" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D64" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="65" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C65" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D65" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="66" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C66" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D66" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="67" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C67" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D67" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="68" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C68" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D68" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="69" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C69" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D69" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="70" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C70" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D70" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="71" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C71" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D71" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="72" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C72" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D72" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="73" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C73" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D73" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="74" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C74" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D74" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="75" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C75" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D75" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="76" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C76" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D76" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="77" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C77" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D77" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="78" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C78" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D78" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="79" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C79" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D79" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="80" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C80" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D80" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="81" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C81" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D81" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="82" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C82" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D82" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="83" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C83" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D83" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="84" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C84" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D84" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="85" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C85" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D85" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="86" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C86" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D86" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="87" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C87" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D87" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="88" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C88" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D88" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="89" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C89" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D89" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="90" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C90" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D90" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="91" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C91" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D91" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="92" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C92" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D92" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="93" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C93" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D93" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="94" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C94" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D94" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="95" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C95" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D95" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="96" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C96" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D96" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="97" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C97" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D97" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="98" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D98" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="99" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D99" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="100" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D100" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="101" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D101" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="102" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D102" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="103" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D103" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="104" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D104" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="105" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D105" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="106" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D106" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="107" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D107" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="108" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D108" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="109" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D109" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="110" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D110" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="111" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D111" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="112" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D112" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="113" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D113" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="114" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D114" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="115" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D115" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="116" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D116" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="117" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D117" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="118" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D118" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="119" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D119" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="120" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D120" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="121" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D121" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="122" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D122" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="123" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D123" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="124" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D124" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="125" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D125" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="126" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D126" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="127" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D127" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="128" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D128" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="129" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D129" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="130" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D130" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="131" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D131" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="132" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D132" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="133" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D133" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="134" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D134" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="135" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D135" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="136" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D136" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="137" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D137" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="138" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D138" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="139" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D139" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="140" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D140" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="141" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D141" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="142" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D142" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="143" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D143" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="144" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D144" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="145" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D145" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="146" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D146" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="147" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D147" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="148" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D148" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="149" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D149" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="150" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D150" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="151" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D151" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="152" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D152" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="153" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D153" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="154" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D154" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="155" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D155" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="156" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D156" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="157" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D157" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="158" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D158" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="159" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D159" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="160" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D160" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="161" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D161" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="162" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D162" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="163" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D163" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="164" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D164" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="165" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D165" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="166" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D166" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="167" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D167" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="168" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D168" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="169" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D169" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="170" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D170" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="171" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D171" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="172" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D172" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="173" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D173" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="174" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D174" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="175" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D175" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="176" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D176" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="177" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D177" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="178" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D178" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="179" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D179" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="180" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D180" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="181" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D181" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="182" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D182" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="183" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D183" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="184" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D184" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="185" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D185" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="186" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D186" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="187" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D187" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="188" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D188" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="189" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D189" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="190" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D190" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="191" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D191" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="192" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D192" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="193" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D193" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="194" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D194" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="195" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D195" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="196" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D196" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="197" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D197" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="198" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D198" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="199" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D199" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="200" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D200" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="201" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D201" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="202" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D202" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="203" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D203" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="204" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D204" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="205" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D205" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="206" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D206" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="207" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D207" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="208" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D208" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="209" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D209" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="210" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D210" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="211" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D211" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="212" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D212" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="213" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D213" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="214" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D214" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="215" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D215" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="216" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D216" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="217" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D217" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="218" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D218" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="219" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D219" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="220" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D220" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="221" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D221" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="222" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D222" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="223" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D223" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="224" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D224" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="225" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D225" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="226" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D226" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="227" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D227" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="228" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D228" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="229" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D229" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="230" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D230" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="231" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D231" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="232" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D232" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="233" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D233" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="234" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D234" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="235" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D235" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="236" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D236" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="237" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D237" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="238" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D238" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="239" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D239" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="240" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D240" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="241" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D241" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="242" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D242" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="243" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D243" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="244" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D244" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="245" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D245" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="246" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D246" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="247" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D247" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="248" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D248" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="249" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D249" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="250" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D250" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="251" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D251" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="252" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D252" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="253" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D253" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="254" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D254" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="255" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D255" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="256" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D256" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="257" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D257" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="258" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D258" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="259" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D259" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="260" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D260" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="261" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D261" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="262" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D262" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="263" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D263" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="264" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D264" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="265" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D265" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="266" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D266" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="267" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D267" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="268" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D268" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="269" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D269" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="270" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D270" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="271" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D271" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="272" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D272" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="273" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D273" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="274" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D274" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="275" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D275" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="276" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D276" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="277" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D277" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="278" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D278" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="279" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D279" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="280" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D280" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="281" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D281" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="282" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D282" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="283" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D283" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="284" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D284" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="285" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D285" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="286" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D286" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="287" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D287" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="288" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D288" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="289" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D289" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="290" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D290" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="291" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D291" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="292" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D292" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="293" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D293" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="294" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D294" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="295" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D295" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="296" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D296" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="297" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D297" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="298" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D298" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="299" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D299" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="300" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D300" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="301" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D301" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="302" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D302" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="303" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D303" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="304" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D304" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="305" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D305" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="306" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D306" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="307" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D307" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="308" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D308" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="309" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D309" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="310" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D310" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="311" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D311" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="312" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D312" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="313" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D313" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="314" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D314" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="315" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D315" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="316" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D316" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="317" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D317" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="318" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D318" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="319" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D319" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="320" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D320" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="321" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D321" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="322" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D322" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="323" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D323" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="324" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D324" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="325" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D325" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="326" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D326" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="327" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D327" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="328" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D328" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="329" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D329" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="330" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D330" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="331" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D331" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="332" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D332" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="333" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D333" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="334" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D334" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="335" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D335" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="336" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D336" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="337" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D337" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="338" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D338" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="339" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D339" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="340" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D340" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="341" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D341" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="342" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D342" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="343" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D343" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="344" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D344" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="345" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D345" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="346" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D346" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="347" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D347" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="348" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D348" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="349" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D349" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="350" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D350" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="351" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D351" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="352" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D352" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="353" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D353" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="354" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D354" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="355" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D355" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="356" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D356" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="357" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D357" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="358" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D358" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="359" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D359" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="360" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D360" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="361" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D361" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="362" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D362" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="363" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D363" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="364" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D364" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="365" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D365" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="366" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D366" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="367" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D367" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="368" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D368" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="369" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D369" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="370" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D370" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="371" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D371" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="372" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D372" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="373" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D373" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="374" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D374" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="375" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D375" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="376" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D376" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="377" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D377" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="378" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D378" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="379" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D379" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="380" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D380" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="381" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D381" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="382" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D382" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="383" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D383" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="384" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D384" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="385" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D385" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="386" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
fixing axiom rename and template
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Experiment_run_AXIOM_v4_6_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Experiment_run_AXIOM_v4_6_0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmarcelino/Desktop/freezeman/backend/fms_core/static/submission_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5357F85D-67D2-9540-8540-3207947F0A17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06E94F34-EB32-CC40-9ABC-19FF41141F85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1660" yWindow="-17560" windowWidth="27040" windowHeight="15780" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-1660" yWindow="-17560" windowWidth="27040" windowHeight="15780" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Experiments" sheetId="1" r:id="rId1"/>
@@ -1470,9 +1470,6 @@
     <t>Axiom</t>
   </si>
   <si>
-    <t>axiom genetitan array</t>
-  </si>
-  <si>
     <t>Protected</t>
   </si>
   <si>
@@ -1480,6 +1477,9 @@
   </si>
   <si>
     <t>Experiment run AXIOM template instructions</t>
+  </si>
+  <si>
+    <t>axiom 96-format  array</t>
   </si>
 </sst>
 </file>
@@ -2170,9 +2170,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O996"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K6" sqref="K6"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2320,7 +2320,7 @@
       <c r="A7" s="33"/>
       <c r="B7" s="2"/>
       <c r="C7" s="31" t="str">
-        <f>IF(A7&lt;&gt;"","axiom genetitan array","")</f>
+        <f>IF(A7&lt;&gt;"","axiom 96-format  array","")</f>
         <v/>
       </c>
       <c r="D7" s="2"/>
@@ -2331,7 +2331,7 @@
       <c r="A8" s="32"/>
       <c r="B8" s="2"/>
       <c r="C8" s="31" t="str">
-        <f t="shared" ref="C8:C26" si="0">IF(A8&lt;&gt;"","axiom genetitan array","")</f>
+        <f t="shared" ref="C8:C26" si="0">IF(A8&lt;&gt;"","axiom 96-format  array","")</f>
         <v/>
       </c>
       <c r="D8" s="2"/>
@@ -19946,7 +19946,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -20200,8 +20200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20247,7 +20247,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
       <c r="B2" t="s">
         <v>27</v>
@@ -20262,7 +20262,7 @@
         <v>60</v>
       </c>
       <c r="F2" s="31" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="G2" s="29" t="s">
         <v>61</v>
@@ -20286,7 +20286,7 @@
         <v>64</v>
       </c>
       <c r="F3" s="31" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="G3" s="29" t="s">
         <v>65</v>

</xml_diff>

<commit_message>
fixing template+cleanup for run
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Experiment_run_AXIOM_v4_6_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Experiment_run_AXIOM_v4_6_0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmarcelino/Desktop/freezeman/backend/fms_core/static/submission_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06E94F34-EB32-CC40-9ABC-19FF41141F85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D0D15F1-1EDF-614C-8FE4-0C871ECE2071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1660" yWindow="-17560" windowWidth="27040" windowHeight="15780" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="27040" windowHeight="17560" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Experiments" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="458">
   <si>
     <t>Experiment Submission Template</t>
   </si>
@@ -210,9 +210,6 @@
     <t>C02</t>
   </si>
   <si>
-    <t>Formula</t>
-  </si>
-  <si>
     <t>Coord</t>
   </si>
   <si>
@@ -1480,6 +1477,21 @@
   </si>
   <si>
     <t>axiom 96-format  array</t>
+  </si>
+  <si>
+    <t>Unique barcode for axiom module 4.1</t>
+  </si>
+  <si>
+    <t>Unique barcode for axiom module 4.2</t>
+  </si>
+  <si>
+    <t>Name of the liquid Handler Instrument</t>
+  </si>
+  <si>
+    <t>Addtitional information for Reagent Preparation</t>
+  </si>
+  <si>
+    <t>Additional information for denaturation and hybridization</t>
   </si>
 </sst>
 </file>
@@ -2170,9 +2182,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O996"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2225,7 +2237,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -10334,9 +10346,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10358,12 +10370,8 @@
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
-      <c r="F1" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="31" t="s">
-        <v>30</v>
-      </c>
+      <c r="F1" s="32"/>
+      <c r="G1" s="31"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
@@ -18466,19 +18474,19 @@
     </row>
     <row r="2" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="C2" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="D2" s="31" t="s">
+        <v>447</v>
+      </c>
+      <c r="E2" t="s">
         <v>33</v>
-      </c>
-      <c r="D2" s="31" t="s">
-        <v>448</v>
-      </c>
-      <c r="E2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -19935,8 +19943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -19946,7 +19954,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -19957,7 +19965,7 @@
     </row>
     <row r="7" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -19965,7 +19973,7 @@
     </row>
     <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B9" s="24"/>
     </row>
@@ -19974,7 +19982,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" s="28"/>
     </row>
@@ -19983,7 +19991,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" s="28"/>
     </row>
@@ -19992,7 +20000,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12" s="28"/>
     </row>
@@ -20001,7 +20009,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C13" s="28"/>
     </row>
@@ -20010,7 +20018,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C14" s="28"/>
     </row>
@@ -20019,7 +20027,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15" s="28"/>
     </row>
@@ -20027,35 +20035,45 @@
       <c r="A16" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="27"/>
+      <c r="B16" s="27" t="s">
+        <v>457</v>
+      </c>
       <c r="C16" s="28"/>
     </row>
     <row r="17" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="27"/>
+      <c r="B17" s="27" t="s">
+        <v>453</v>
+      </c>
       <c r="C17" s="28"/>
     </row>
     <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="27"/>
+      <c r="B18" s="27" t="s">
+        <v>454</v>
+      </c>
       <c r="C18" s="28"/>
     </row>
     <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="27"/>
+      <c r="B19" s="27" t="s">
+        <v>455</v>
+      </c>
       <c r="C19" s="28"/>
     </row>
     <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="27"/>
+      <c r="B20" s="27" t="s">
+        <v>456</v>
+      </c>
       <c r="C20" s="28"/>
     </row>
     <row r="21" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -20100,7 +20118,7 @@
     </row>
     <row r="29" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B29" s="29"/>
       <c r="C29" s="29"/>
@@ -20110,7 +20128,7 @@
         <v>8</v>
       </c>
       <c r="B30" s="27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C30" s="28"/>
     </row>
@@ -20119,7 +20137,7 @@
         <v>20</v>
       </c>
       <c r="B31" s="27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C31" s="28"/>
     </row>
@@ -20128,7 +20146,7 @@
         <v>21</v>
       </c>
       <c r="B32" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C32" s="28"/>
     </row>
@@ -20137,16 +20155,16 @@
         <v>22</v>
       </c>
       <c r="B33" s="27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C33" s="28"/>
     </row>
     <row r="34" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34" s="27" t="s">
         <v>49</v>
-      </c>
-      <c r="B34" s="27" t="s">
-        <v>50</v>
       </c>
       <c r="C34" s="28"/>
     </row>
@@ -20155,7 +20173,7 @@
         <v>24</v>
       </c>
       <c r="B35" s="27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C35" s="28"/>
     </row>
@@ -20164,7 +20182,7 @@
         <v>25</v>
       </c>
       <c r="B36" s="27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C36" s="28"/>
     </row>
@@ -20173,7 +20191,7 @@
         <v>13</v>
       </c>
       <c r="B37" s="27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C37" s="28"/>
     </row>
@@ -20182,7 +20200,7 @@
         <v>26</v>
       </c>
       <c r="B38" s="27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C38" s="28"/>
     </row>
@@ -20221,25 +20239,25 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
         <v>55</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>56</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>57</v>
       </c>
-      <c r="D1" t="s">
-        <v>58</v>
-      </c>
       <c r="E1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F1" t="s">
         <v>11</v>
       </c>
       <c r="G1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J1" t="s">
         <v>26</v>
@@ -20247,7 +20265,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B2" t="s">
         <v>27</v>
@@ -20259,129 +20277,129 @@
         <v>27</v>
       </c>
       <c r="E2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="31" t="s">
+        <v>449</v>
+      </c>
+      <c r="G2" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="F2" s="31" t="s">
-        <v>450</v>
-      </c>
-      <c r="G2" s="29" t="s">
+      <c r="J2" t="s">
         <v>61</v>
-      </c>
-      <c r="J2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="24"/>
       <c r="B3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" t="s">
         <v>63</v>
       </c>
-      <c r="C3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F3" s="31" t="s">
+        <v>450</v>
+      </c>
+      <c r="G3" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="F3" s="31" t="s">
-        <v>451</v>
-      </c>
-      <c r="G3" s="29" t="s">
+      <c r="J3" t="s">
         <v>65</v>
-      </c>
-      <c r="J3" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" t="s">
+        <v>66</v>
+      </c>
+      <c r="J4" t="s">
         <v>67</v>
-      </c>
-      <c r="C4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4" t="s">
-        <v>67</v>
-      </c>
-      <c r="J4" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
@@ -20389,100 +20407,100 @@
         <v>28</v>
       </c>
       <c r="D14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15" t="s">
         <v>79</v>
-      </c>
-      <c r="D15" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" t="s">
         <v>81</v>
-      </c>
-      <c r="D16" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" t="s">
         <v>83</v>
-      </c>
-      <c r="D17" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
+        <v>84</v>
+      </c>
+      <c r="D18" t="s">
         <v>85</v>
-      </c>
-      <c r="D18" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C19" t="s">
+        <v>86</v>
+      </c>
+      <c r="D19" t="s">
         <v>87</v>
-      </c>
-      <c r="D19" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="20" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C20" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20" t="s">
         <v>89</v>
-      </c>
-      <c r="D20" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="21" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C21" t="s">
+        <v>90</v>
+      </c>
+      <c r="D21" t="s">
         <v>91</v>
-      </c>
-      <c r="D21" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="22" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C22" t="s">
+        <v>92</v>
+      </c>
+      <c r="D22" t="s">
         <v>93</v>
-      </c>
-      <c r="D22" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="23" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C23" t="s">
+        <v>94</v>
+      </c>
+      <c r="D23" t="s">
         <v>95</v>
-      </c>
-      <c r="D23" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="24" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
+        <v>96</v>
+      </c>
+      <c r="D24" t="s">
         <v>97</v>
-      </c>
-      <c r="D24" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="25" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
+        <v>98</v>
+      </c>
+      <c r="D25" t="s">
         <v>99</v>
-      </c>
-      <c r="D25" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="26" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D26" t="s">
         <v>28</v>
@@ -20493,196 +20511,196 @@
         <v>29</v>
       </c>
       <c r="D27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C28" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D28" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C29" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C30" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D30" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D31" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C32" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D32" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C33" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D33" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C34" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D34" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="35" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C35" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D35" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="36" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D36" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="37" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C37" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D37" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="38" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C38" t="s">
+        <v>111</v>
+      </c>
+      <c r="D38" t="s">
         <v>112</v>
-      </c>
-      <c r="D38" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="39" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C39" t="s">
+        <v>113</v>
+      </c>
+      <c r="D39" t="s">
         <v>114</v>
-      </c>
-      <c r="D39" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="40" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C40" t="s">
+        <v>115</v>
+      </c>
+      <c r="D40" t="s">
         <v>116</v>
-      </c>
-      <c r="D40" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="41" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C41" t="s">
+        <v>117</v>
+      </c>
+      <c r="D41" t="s">
         <v>118</v>
-      </c>
-      <c r="D41" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="42" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C42" t="s">
+        <v>119</v>
+      </c>
+      <c r="D42" t="s">
         <v>120</v>
-      </c>
-      <c r="D42" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="43" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C43" t="s">
+        <v>121</v>
+      </c>
+      <c r="D43" t="s">
         <v>122</v>
-      </c>
-      <c r="D43" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="44" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C44" t="s">
+        <v>123</v>
+      </c>
+      <c r="D44" t="s">
         <v>124</v>
-      </c>
-      <c r="D44" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="45" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C45" t="s">
+        <v>125</v>
+      </c>
+      <c r="D45" t="s">
         <v>126</v>
-      </c>
-      <c r="D45" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="46" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C46" t="s">
+        <v>127</v>
+      </c>
+      <c r="D46" t="s">
         <v>128</v>
-      </c>
-      <c r="D46" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="47" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C47" t="s">
+        <v>129</v>
+      </c>
+      <c r="D47" t="s">
         <v>130</v>
-      </c>
-      <c r="D47" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="48" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C48" t="s">
+        <v>131</v>
+      </c>
+      <c r="D48" t="s">
         <v>132</v>
-      </c>
-      <c r="D48" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="49" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C49" t="s">
+        <v>133</v>
+      </c>
+      <c r="D49" t="s">
         <v>134</v>
-      </c>
-      <c r="D49" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="50" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C50" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D50" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="51" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C51" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D51" t="s">
         <v>29</v>
@@ -20690,1810 +20708,1810 @@
     </row>
     <row r="52" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C52" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D52" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="53" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C53" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D53" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="54" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C54" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D54" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="55" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C55" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D55" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="56" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C56" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D56" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="57" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C57" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D57" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="58" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C58" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D58" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="59" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C59" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D59" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="60" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C60" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D60" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="61" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C61" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D61" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="62" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C62" t="s">
+        <v>147</v>
+      </c>
+      <c r="D62" t="s">
         <v>148</v>
-      </c>
-      <c r="D62" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="63" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C63" t="s">
+        <v>149</v>
+      </c>
+      <c r="D63" t="s">
         <v>150</v>
-      </c>
-      <c r="D63" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="64" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C64" t="s">
+        <v>151</v>
+      </c>
+      <c r="D64" t="s">
         <v>152</v>
-      </c>
-      <c r="D64" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="65" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C65" t="s">
+        <v>153</v>
+      </c>
+      <c r="D65" t="s">
         <v>154</v>
-      </c>
-      <c r="D65" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="66" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C66" t="s">
+        <v>155</v>
+      </c>
+      <c r="D66" t="s">
         <v>156</v>
-      </c>
-      <c r="D66" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="67" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C67" t="s">
+        <v>157</v>
+      </c>
+      <c r="D67" t="s">
         <v>158</v>
-      </c>
-      <c r="D67" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="68" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C68" t="s">
+        <v>159</v>
+      </c>
+      <c r="D68" t="s">
         <v>160</v>
-      </c>
-      <c r="D68" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="69" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C69" t="s">
+        <v>161</v>
+      </c>
+      <c r="D69" t="s">
         <v>162</v>
-      </c>
-      <c r="D69" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="70" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C70" t="s">
+        <v>163</v>
+      </c>
+      <c r="D70" t="s">
         <v>164</v>
-      </c>
-      <c r="D70" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="71" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C71" t="s">
+        <v>165</v>
+      </c>
+      <c r="D71" t="s">
         <v>166</v>
-      </c>
-      <c r="D71" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="72" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C72" t="s">
+        <v>167</v>
+      </c>
+      <c r="D72" t="s">
         <v>168</v>
-      </c>
-      <c r="D72" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="73" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C73" t="s">
+        <v>169</v>
+      </c>
+      <c r="D73" t="s">
         <v>170</v>
-      </c>
-      <c r="D73" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="74" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C74" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D74" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="75" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C75" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D75" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="76" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C76" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D76" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="77" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C77" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D77" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="78" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C78" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D78" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="79" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C79" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D79" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="80" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C80" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D80" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="81" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C81" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D81" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="82" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C82" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D82" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="83" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C83" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D83" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="84" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C84" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D84" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="85" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C85" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D85" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="86" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C86" t="s">
+        <v>183</v>
+      </c>
+      <c r="D86" t="s">
         <v>184</v>
-      </c>
-      <c r="D86" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="87" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C87" t="s">
+        <v>185</v>
+      </c>
+      <c r="D87" t="s">
         <v>186</v>
-      </c>
-      <c r="D87" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="88" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C88" t="s">
+        <v>187</v>
+      </c>
+      <c r="D88" t="s">
         <v>188</v>
-      </c>
-      <c r="D88" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="89" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C89" t="s">
+        <v>189</v>
+      </c>
+      <c r="D89" t="s">
         <v>190</v>
-      </c>
-      <c r="D89" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="90" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C90" t="s">
+        <v>191</v>
+      </c>
+      <c r="D90" t="s">
         <v>192</v>
-      </c>
-      <c r="D90" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="91" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C91" t="s">
+        <v>193</v>
+      </c>
+      <c r="D91" t="s">
         <v>194</v>
-      </c>
-      <c r="D91" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="92" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C92" t="s">
+        <v>195</v>
+      </c>
+      <c r="D92" t="s">
         <v>196</v>
-      </c>
-      <c r="D92" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="93" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C93" t="s">
+        <v>197</v>
+      </c>
+      <c r="D93" t="s">
         <v>198</v>
-      </c>
-      <c r="D93" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="94" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C94" t="s">
+        <v>199</v>
+      </c>
+      <c r="D94" t="s">
         <v>200</v>
-      </c>
-      <c r="D94" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="95" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C95" t="s">
+        <v>201</v>
+      </c>
+      <c r="D95" t="s">
         <v>202</v>
-      </c>
-      <c r="D95" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="96" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C96" t="s">
+        <v>203</v>
+      </c>
+      <c r="D96" t="s">
         <v>204</v>
-      </c>
-      <c r="D96" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="97" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C97" t="s">
+        <v>205</v>
+      </c>
+      <c r="D97" t="s">
         <v>206</v>
-      </c>
-      <c r="D97" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="98" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D98" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="99" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D99" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="100" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D100" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="101" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D101" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="102" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D102" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="103" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D103" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="104" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D104" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="105" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D105" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="106" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D106" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="107" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D107" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="108" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D108" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="109" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D109" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="110" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D110" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="111" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D111" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="112" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D112" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="113" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D113" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="114" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D114" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="115" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D115" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="116" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D116" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="117" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D117" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="118" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D118" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="119" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D119" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="120" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D120" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="121" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D121" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="122" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D122" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="123" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D123" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="124" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D124" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="125" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D125" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="126" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D126" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="127" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D127" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="128" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D128" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="129" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D129" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="130" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D130" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="131" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D131" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="132" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D132" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="133" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D133" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="134" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D134" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="135" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D135" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="136" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D136" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="137" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D137" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="138" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D138" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="139" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D139" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="140" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D140" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="141" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D141" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="142" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D142" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="143" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D143" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="144" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D144" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="145" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D145" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="146" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D146" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="147" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D147" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="148" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D148" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="149" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D149" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="150" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D150" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="151" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D151" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="152" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D152" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="153" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D153" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="154" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D154" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="155" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D155" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="156" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D156" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="157" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D157" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="158" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D158" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="159" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D159" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="160" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D160" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="161" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D161" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="162" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D162" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="163" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D163" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="164" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D164" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="165" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D165" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="166" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D166" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="167" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D167" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="168" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D168" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="169" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D169" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="170" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D170" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="171" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D171" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="172" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D172" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="173" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D173" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="174" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D174" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="175" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D175" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="176" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D176" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="177" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D177" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="178" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D178" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="179" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D179" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="180" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D180" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="181" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D181" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="182" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D182" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="183" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D183" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="184" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D184" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="185" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D185" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="186" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D186" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="187" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D187" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="188" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D188" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="189" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D189" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="190" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D190" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="191" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D191" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="192" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D192" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="193" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D193" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="194" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D194" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="195" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D195" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="196" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D196" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="197" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D197" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="198" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D198" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="199" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D199" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="200" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D200" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="201" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D201" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="202" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D202" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="203" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D203" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="204" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D204" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="205" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D205" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="206" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D206" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="207" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D207" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="208" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D208" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="209" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D209" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="210" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D210" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="211" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D211" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="212" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D212" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="213" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D213" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="214" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D214" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="215" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D215" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="216" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D216" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="217" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D217" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="218" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D218" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="219" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D219" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="220" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D220" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="221" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D221" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="222" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D222" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="223" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D223" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="224" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D224" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="225" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D225" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="226" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D226" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="227" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D227" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="228" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D228" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="229" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D229" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="230" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D230" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="231" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D231" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="232" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D232" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="233" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D233" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="234" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D234" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="235" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D235" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="236" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D236" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="237" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D237" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="238" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D238" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="239" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D239" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="240" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D240" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="241" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D241" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="242" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D242" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="243" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D243" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="244" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D244" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="245" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D245" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="246" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D246" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="247" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D247" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="248" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D248" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="249" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D249" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="250" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D250" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="251" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D251" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="252" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D252" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="253" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D253" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="254" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D254" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="255" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D255" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="256" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D256" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="257" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D257" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="258" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D258" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="259" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D259" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="260" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D260" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="261" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D261" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="262" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D262" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="263" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D263" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="264" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D264" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="265" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D265" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="266" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D266" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="267" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D267" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="268" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D268" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="269" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D269" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="270" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D270" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="271" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D271" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="272" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D272" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="273" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D273" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="274" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D274" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="275" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D275" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="276" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D276" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="277" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D277" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="278" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D278" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="279" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D279" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="280" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D280" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="281" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D281" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="282" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D282" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="283" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D283" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="284" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D284" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="285" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D285" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="286" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D286" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="287" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D287" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="288" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D288" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="289" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D289" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="290" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D290" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="291" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D291" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="292" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D292" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="293" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D293" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="294" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D294" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="295" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D295" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="296" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D296" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="297" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D297" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="298" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D298" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="299" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D299" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="300" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D300" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="301" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D301" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="302" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D302" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="303" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D303" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="304" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D304" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="305" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D305" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="306" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D306" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="307" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D307" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="308" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D308" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="309" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D309" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="310" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D310" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="311" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D311" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="312" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D312" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="313" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D313" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="314" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D314" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="315" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D315" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="316" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D316" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="317" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D317" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="318" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D318" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="319" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D319" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="320" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D320" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="321" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D321" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="322" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D322" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="323" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D323" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="324" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D324" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="325" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D325" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="326" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D326" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="327" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D327" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="328" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D328" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="329" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D329" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="330" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D330" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="331" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D331" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="332" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D332" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="333" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D333" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="334" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D334" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="335" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D335" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="336" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D336" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="337" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D337" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="338" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D338" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="339" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D339" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="340" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D340" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="341" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D341" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="342" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D342" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="343" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D343" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="344" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D344" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="345" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D345" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="346" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D346" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="347" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D347" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="348" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D348" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="349" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D349" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="350" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D350" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="351" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D351" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="352" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D352" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="353" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D353" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="354" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D354" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="355" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D355" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="356" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D356" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="357" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D357" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="358" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D358" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="359" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D359" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="360" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D360" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="361" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D361" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="362" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D362" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="363" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D363" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="364" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D364" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="365" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D365" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="366" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D366" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="367" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D367" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="368" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D368" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="369" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D369" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="370" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D370" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="371" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D371" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="372" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D372" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="373" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D373" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="374" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D374" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="375" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D375" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="376" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D376" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="377" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D377" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="378" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D378" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="379" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D379" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="380" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D380" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="381" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D381" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="382" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D382" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="383" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D383" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="384" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D384" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="385" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D385" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="386" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>